<commit_message>
Se actualizaron los casos del 7 al 10 con la data de excel
</commit_message>
<xml_diff>
--- a/src/test/resources/data/data.xlsx
+++ b/src/test/resources/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Brayan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WIN 20\Desktop\DesafioBootcamp\Desafio_Bootcamp_TSOFT_Grupo2\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79506DF6-A836-4359-BD7E-EBD720C17B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CF01FD-D781-41BF-B2A2-7C93B34D4DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ABFCA762-9C05-4D08-B931-9CB2A8182F8B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ABFCA762-9C05-4D08-B931-9CB2A8182F8B}"/>
   </bookViews>
   <sheets>
     <sheet name="DataPrueba" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="62">
   <si>
     <t>TC018_</t>
   </si>
@@ -62,18 +60,6 @@
     <t>TC011_</t>
   </si>
   <si>
-    <t>TC010_</t>
-  </si>
-  <si>
-    <t>TC009_</t>
-  </si>
-  <si>
-    <t>TC008_</t>
-  </si>
-  <si>
-    <t>TC007_</t>
-  </si>
-  <si>
     <t>TC006_</t>
   </si>
   <si>
@@ -186,6 +172,54 @@
   </si>
   <si>
     <t xml:space="preserve">Tokio </t>
+  </si>
+  <si>
+    <t>TC007_BusquedaDeTrenes_SoloIda</t>
+  </si>
+  <si>
+    <t>Alicante</t>
+  </si>
+  <si>
+    <t>Sevilla</t>
+  </si>
+  <si>
+    <t>Barcelona</t>
+  </si>
+  <si>
+    <t>TC008_BusquedaDeTrenes_IdaYVuelta</t>
+  </si>
+  <si>
+    <t>TC0009_BusquedaDeTrenes_IdaYVuelta_MasRapido_IdaYVueltaAlMismoTiempo</t>
+  </si>
+  <si>
+    <t>TC0010_BusquedaDeTrenes_IdaYVuelta_MasRapido_ReservarAsistenciaEspecial_ModalidadReducida</t>
+  </si>
+  <si>
+    <t>Ciudad Real</t>
+  </si>
+  <si>
+    <t>Córdoba</t>
+  </si>
+  <si>
+    <t>//button[text()='24']</t>
+  </si>
+  <si>
+    <t>//button[text()='19']</t>
+  </si>
+  <si>
+    <t>//button[text()='17']</t>
+  </si>
+  <si>
+    <t>Dylan</t>
+  </si>
+  <si>
+    <t>Huarcaya</t>
+  </si>
+  <si>
+    <t>//span[text()='enero']</t>
+  </si>
+  <si>
+    <t>65004204V</t>
   </si>
 </sst>
 </file>
@@ -258,9 +292,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -298,7 +332,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -404,7 +438,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -546,7 +580,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -556,80 +590,80 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E8DCD68-5826-40B3-86F2-BD2B9C3E6AD7}">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="107.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="107.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -645,22 +679,22 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D3" s="2">
         <v>13</v>
       </c>
       <c r="E3" s="2" t="str">
         <f ca="1">TEXT(TEXT(DAY(TODAY()), "dd")+1, "dd")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1" t="str">
         <f ca="1">TEXT(TODAY(), "mm")</f>
@@ -680,24 +714,24 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -710,15 +744,15 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D5" s="1">
         <v>15</v>
@@ -744,30 +778,30 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -778,9 +812,9 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -798,13 +832,19 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+        <v>46</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -818,14 +858,22 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -838,14 +886,22 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -858,27 +914,47 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="1">
+        <v>16</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11" s="1">
+        <v>2003</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -898,7 +974,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -918,7 +994,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -938,7 +1014,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -958,7 +1034,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -978,7 +1054,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -998,7 +1074,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
@@ -1018,7 +1094,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
-m "Add: Se añadieron funciones en TrenesPage. Se culmino TC0012. Se realizaron optimizaciones en VuelosPage y Cps"
</commit_message>
<xml_diff>
--- a/src/test/resources/data/data.xlsx
+++ b/src/test/resources/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Brayan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pc\Documents\ArchivoClonado\Desafio_Bootcamp_TSOFT_Grupo2\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79506DF6-A836-4359-BD7E-EBD720C17B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4006E8E8-F0ED-4A44-977A-4782273F9341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ABFCA762-9C05-4D08-B931-9CB2A8182F8B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{ABFCA762-9C05-4D08-B931-9CB2A8182F8B}"/>
   </bookViews>
   <sheets>
     <sheet name="DataPrueba" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>TC018_</t>
   </si>
@@ -56,9 +45,6 @@
     <t>TC013_</t>
   </si>
   <si>
-    <t>TC012_</t>
-  </si>
-  <si>
     <t>TC011_</t>
   </si>
   <si>
@@ -186,6 +172,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tokio </t>
+  </si>
+  <si>
+    <t>TC0012_Filtrado_Trenes_MAD_VLC_Precio_Equipaje_Escala_Salida_Aere_Esta</t>
   </si>
 </sst>
 </file>
@@ -258,9 +247,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -298,7 +287,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -404,7 +393,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -546,7 +535,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -557,79 +546,79 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="107.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="107.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -645,22 +634,22 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="D3" s="2">
         <v>13</v>
       </c>
       <c r="E3" s="2" t="str">
         <f ca="1">TEXT(TEXT(DAY(TODAY()), "dd")+1, "dd")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1" t="str">
         <f ca="1">TEXT(TODAY(), "mm")</f>
@@ -680,24 +669,24 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -710,15 +699,15 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="D5" s="1">
         <v>15</v>
@@ -744,30 +733,30 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -778,9 +767,9 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -798,9 +787,9 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -818,9 +807,9 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -838,9 +827,9 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -858,9 +847,9 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -878,9 +867,9 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -898,14 +887,22 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1">
+        <v>20</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -918,7 +915,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -938,7 +935,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -958,7 +955,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -978,7 +975,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -998,7 +995,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
@@ -1018,7 +1015,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Agregar datos al Excel para las prueba TC0012
</commit_message>
<xml_diff>
--- a/src/test/resources/data/data.xlsx
+++ b/src/test/resources/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WIN 20\Desktop\DesafioBootcamp\Desafio_Bootcamp_TSOFT_Grupo2\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tsoft\desafio\Desafio_Bootcamp_TSOFT_Grupo2\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CF01FD-D781-41BF-B2A2-7C93B34D4DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1616899C-E9ED-4661-BE7F-5E22C03A8174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ABFCA762-9C05-4D08-B931-9CB2A8182F8B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ABFCA762-9C05-4D08-B931-9CB2A8182F8B}"/>
   </bookViews>
   <sheets>
     <sheet name="DataPrueba" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
   <si>
     <t>TC018_</t>
   </si>
@@ -54,9 +54,6 @@
     <t>TC013_</t>
   </si>
   <si>
-    <t>TC012_</t>
-  </si>
-  <si>
     <t>TC011_</t>
   </si>
   <si>
@@ -220,6 +217,9 @@
   </si>
   <si>
     <t>65004204V</t>
+  </si>
+  <si>
+    <t>TC0012_Filtrado_Trenes_MAD_VLC_Precio_Equipaje_Escala_Salida_Aere_Esta</t>
   </si>
 </sst>
 </file>
@@ -292,9 +292,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -332,7 +332,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -438,7 +438,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -580,7 +580,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -590,80 +590,80 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E8DCD68-5826-40B3-86F2-BD2B9C3E6AD7}">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="107.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="107.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -679,15 +679,15 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="D3" s="2">
         <v>13</v>
@@ -714,24 +714,24 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -744,15 +744,15 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="D5" s="1">
         <v>15</v>
@@ -778,30 +778,30 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -812,9 +812,9 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -832,18 +832,18 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -858,21 +858,21 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -886,21 +886,21 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -914,39 +914,39 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="H11" s="1">
         <v>16</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J11" s="1">
         <v>2003</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -954,9 +954,9 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -974,14 +974,22 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="1">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1">
+        <v>20</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -994,7 +1002,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -1014,7 +1022,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1034,7 +1042,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -1054,7 +1062,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1074,7 +1082,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
@@ -1094,7 +1102,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Actualizar datos del Excel para la prueba TC005
</commit_message>
<xml_diff>
--- a/src/test/resources/data/data.xlsx
+++ b/src/test/resources/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tsoft\desafio\Desafio_Bootcamp_TSOFT_Grupo2\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1616899C-E9ED-4661-BE7F-5E22C03A8174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D2D347-5AF8-4024-9F20-B65F7B8981B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ABFCA762-9C05-4D08-B931-9CB2A8182F8B}"/>
   </bookViews>
@@ -69,9 +69,6 @@
     <t>Introduce el apellido</t>
   </si>
   <si>
-    <t>Introduce el nombre</t>
-  </si>
-  <si>
     <t>//div[@aria-labelledby='5-2024']//button[text()='8']</t>
   </si>
   <si>
@@ -220,6 +217,9 @@
   </si>
   <si>
     <t>TC0012_Filtrado_Trenes_MAD_VLC_Precio_Equipaje_Escala_Salida_Aere_Esta</t>
+  </si>
+  <si>
+    <t>Introduce el nombre y cualquier segundo nombre.</t>
   </si>
 </sst>
 </file>
@@ -590,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E8DCD68-5826-40B3-86F2-BD2B9C3E6AD7}">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,63 +607,63 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -681,20 +681,20 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="D3" s="2">
         <v>13</v>
       </c>
       <c r="E3" s="2" t="str">
         <f ca="1">TEXT(TEXT(DAY(TODAY()), "dd")+1, "dd")</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" s="1" t="str">
         <f ca="1">TEXT(TODAY(), "mm")</f>
@@ -716,22 +716,22 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -746,13 +746,13 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="D5" s="1">
         <v>15</v>
@@ -780,19 +780,19 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>10</v>
@@ -834,16 +834,16 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -860,19 +860,19 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -888,19 +888,19 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -916,37 +916,37 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="H11" s="1">
         <v>16</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J11" s="1">
         <v>2003</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -976,13 +976,13 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="D13" s="1">
         <v>16</v>

</xml_diff>